<commit_message>
separate data and code
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,14 +476,30 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>日</t>
+          <t>火</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>清水在宅作業</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1:00</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -491,7 +507,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>月</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -502,12 +518,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>09:06</t>
+          <t>09:37</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>18:06</t>
+          <t>18:37</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -522,7 +538,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -533,12 +549,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>10:20</t>
+          <t>09:01</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>19:22</t>
+          <t>18:26</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -553,7 +569,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>水</t>
+          <t>金</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -564,12 +580,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>09:20</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>18:29</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -584,30 +600,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>木</t>
+          <t>土</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>清水在宅作業</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>09:19</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>18:30</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>1:00</t>
-        </is>
-      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -615,30 +615,14 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>金</t>
+          <t>日</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>清水在宅作業</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>10:01</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>19:01</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>1:00</t>
-        </is>
-      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -646,14 +630,30 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>土</t>
+          <t>月</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>清水在宅作業</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>18:40</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1:00</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -661,14 +661,30 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>日</t>
+          <t>火</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>清水在宅作業</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>20:01</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1:00</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -676,7 +692,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>月</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -687,12 +703,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>09:02</t>
+          <t>09:06</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>18:06</t>
+          <t>19:03</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -707,7 +723,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -718,12 +734,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>09:51</t>
+          <t>09:18</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>18:51</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -738,7 +754,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>水</t>
+          <t>金</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -749,12 +765,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>09:06</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>18:16</t>
+          <t>18:17</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -769,30 +785,14 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>木</t>
+          <t>土</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>清水在宅作業</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>09:04</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>18:17</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>1:00</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -800,26 +800,14 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>金</t>
+          <t>日</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>清水在宅作業</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>09:51</t>
-        </is>
-      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>1:00</t>
-        </is>
-      </c>
+      <c r="G14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -827,14 +815,30 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>土</t>
+          <t>月</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>清水在宅作業</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>09:29</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>18:38</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>1:00</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -842,14 +846,30 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>日</t>
+          <t>火</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>清水在宅作業</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>09:12</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>18:36</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>1:00</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -857,7 +877,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>月</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -868,12 +888,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>09:03</t>
+          <t>09:30</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:30</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -888,7 +908,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -899,12 +919,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>09:46</t>
+          <t>09:41</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -919,7 +939,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>水</t>
+          <t>金</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
@@ -930,12 +950,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>09:05</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -950,30 +970,14 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>木</t>
+          <t>土</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>清水在宅作業</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>09:16</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>18:30</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>1:00</t>
-        </is>
-      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -981,30 +985,14 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>金</t>
+          <t>日</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>清水在宅作業</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>09:30</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>19:37</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>1:00</t>
-        </is>
-      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1012,7 +1000,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>土</t>
+          <t>月</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -1027,14 +1015,30 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>日</t>
+          <t>火</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>清水在宅作業</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>10:31</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>20:04</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>1:00</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1042,7 +1046,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>月</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -1053,12 +1057,12 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>10:50</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>18:47</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1073,7 +1077,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
@@ -1084,12 +1088,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:31</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>16:12</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1104,7 +1108,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>水</t>
+          <t>金</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -1115,12 +1119,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>09:48</t>
+          <t>11:01</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>18:50</t>
+          <t>20:04</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1135,7 +1139,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>木</t>
+          <t>土</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
@@ -1150,30 +1154,14 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>金</t>
+          <t>日</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>清水在宅作業</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>19:31</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>1:00</t>
-        </is>
-      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1181,14 +1169,30 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>土</t>
+          <t>月</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>清水在宅作業</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>09:24</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>18:29</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>1:00</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1196,14 +1200,30 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>日</t>
+          <t>火</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>清水在宅作業</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>1:00</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1211,7 +1231,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>月</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
@@ -1222,11 +1242,46 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>09:56</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr"/>
+          <t>09:06</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
       <c r="G31" t="inlineStr">
+        <is>
+          <t>1:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>木</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>清水在宅作業</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>09:06</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>18:18</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
         <is>
           <t>1:00</t>
         </is>

</xml_diff>